<commit_message>
activity_relation_data_stats: add analysis of branch lengths and nested gateways
</commit_message>
<xml_diff>
--- a/data/paper_stats/activity_relation/activity_relation_data_stats.xlsx
+++ b/data/paper_stats/activity_relation/activity_relation_data_stats.xlsx
@@ -9,7 +9,8 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Relation Type Count" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Comment Count" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Doc Stats" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Doc Count" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Doc Stats" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -490,16 +491,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C2" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E2" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
@@ -509,16 +510,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C3" t="n">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D3" t="n">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E3" t="n">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="4">
@@ -528,16 +529,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>446</v>
+        <v>470</v>
       </c>
       <c r="C4" t="n">
-        <v>446</v>
+        <v>470</v>
       </c>
       <c r="D4" t="n">
-        <v>446</v>
+        <v>470</v>
       </c>
       <c r="E4" t="n">
-        <v>446</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -598,13 +599,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E2" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
@@ -687,13 +688,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D7" t="n">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E7" t="n">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8">
@@ -708,13 +709,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>446</v>
+        <v>470</v>
       </c>
       <c r="D8" t="n">
-        <v>446</v>
+        <v>470</v>
       </c>
       <c r="E8" t="n">
-        <v>446</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -726,6 +727,888 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>doc_name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>gateway_1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>gateway_2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>relation_type</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>doc-1.1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>26</v>
+      </c>
+      <c r="C2" t="n">
+        <v>26</v>
+      </c>
+      <c r="D2" t="n">
+        <v>26</v>
+      </c>
+      <c r="E2" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>doc-1.2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" t="n">
+        <v>20</v>
+      </c>
+      <c r="D3" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>doc-1.3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>13</v>
+      </c>
+      <c r="C4" t="n">
+        <v>13</v>
+      </c>
+      <c r="D4" t="n">
+        <v>13</v>
+      </c>
+      <c r="E4" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>doc-1.4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>13</v>
+      </c>
+      <c r="C5" t="n">
+        <v>13</v>
+      </c>
+      <c r="D5" t="n">
+        <v>13</v>
+      </c>
+      <c r="E5" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.1</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.10</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>15</v>
+      </c>
+      <c r="C7" t="n">
+        <v>15</v>
+      </c>
+      <c r="D7" t="n">
+        <v>15</v>
+      </c>
+      <c r="E7" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.11</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>18</v>
+      </c>
+      <c r="C8" t="n">
+        <v>18</v>
+      </c>
+      <c r="D8" t="n">
+        <v>18</v>
+      </c>
+      <c r="E8" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.12</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.13</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.14</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>37</v>
+      </c>
+      <c r="C11" t="n">
+        <v>37</v>
+      </c>
+      <c r="D11" t="n">
+        <v>37</v>
+      </c>
+      <c r="E11" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.2</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>65</v>
+      </c>
+      <c r="C12" t="n">
+        <v>65</v>
+      </c>
+      <c r="D12" t="n">
+        <v>65</v>
+      </c>
+      <c r="E12" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.3</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>19</v>
+      </c>
+      <c r="C13" t="n">
+        <v>19</v>
+      </c>
+      <c r="D13" t="n">
+        <v>19</v>
+      </c>
+      <c r="E13" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.4</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>11</v>
+      </c>
+      <c r="C14" t="n">
+        <v>11</v>
+      </c>
+      <c r="D14" t="n">
+        <v>11</v>
+      </c>
+      <c r="E14" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.5</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" t="n">
+        <v>4</v>
+      </c>
+      <c r="D15" t="n">
+        <v>4</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.6</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" t="n">
+        <v>4</v>
+      </c>
+      <c r="E16" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.7</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>12</v>
+      </c>
+      <c r="C17" t="n">
+        <v>12</v>
+      </c>
+      <c r="D17" t="n">
+        <v>12</v>
+      </c>
+      <c r="E17" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.8</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>9</v>
+      </c>
+      <c r="C18" t="n">
+        <v>9</v>
+      </c>
+      <c r="D18" t="n">
+        <v>9</v>
+      </c>
+      <c r="E18" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.9</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>12</v>
+      </c>
+      <c r="C19" t="n">
+        <v>12</v>
+      </c>
+      <c r="D19" t="n">
+        <v>12</v>
+      </c>
+      <c r="E19" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>doc-2.1</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>119</v>
+      </c>
+      <c r="C20" t="n">
+        <v>119</v>
+      </c>
+      <c r="D20" t="n">
+        <v>119</v>
+      </c>
+      <c r="E20" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>doc-2.2</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>182</v>
+      </c>
+      <c r="C21" t="n">
+        <v>182</v>
+      </c>
+      <c r="D21" t="n">
+        <v>182</v>
+      </c>
+      <c r="E21" t="n">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>doc-3.1</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>10</v>
+      </c>
+      <c r="C22" t="n">
+        <v>10</v>
+      </c>
+      <c r="D22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E22" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>doc-3.2</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>10</v>
+      </c>
+      <c r="C23" t="n">
+        <v>10</v>
+      </c>
+      <c r="D23" t="n">
+        <v>10</v>
+      </c>
+      <c r="E23" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>doc-3.3</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>11</v>
+      </c>
+      <c r="C24" t="n">
+        <v>11</v>
+      </c>
+      <c r="D24" t="n">
+        <v>11</v>
+      </c>
+      <c r="E24" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>doc-3.5</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>34</v>
+      </c>
+      <c r="C25" t="n">
+        <v>34</v>
+      </c>
+      <c r="D25" t="n">
+        <v>34</v>
+      </c>
+      <c r="E25" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>doc-3.6</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>18</v>
+      </c>
+      <c r="C26" t="n">
+        <v>18</v>
+      </c>
+      <c r="D26" t="n">
+        <v>18</v>
+      </c>
+      <c r="E26" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>doc-3.7</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>5</v>
+      </c>
+      <c r="C27" t="n">
+        <v>5</v>
+      </c>
+      <c r="D27" t="n">
+        <v>5</v>
+      </c>
+      <c r="E27" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>doc-3.8</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>12</v>
+      </c>
+      <c r="C28" t="n">
+        <v>12</v>
+      </c>
+      <c r="D28" t="n">
+        <v>12</v>
+      </c>
+      <c r="E28" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>doc-4.1</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>37</v>
+      </c>
+      <c r="C29" t="n">
+        <v>37</v>
+      </c>
+      <c r="D29" t="n">
+        <v>37</v>
+      </c>
+      <c r="E29" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>doc-5.1</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>10</v>
+      </c>
+      <c r="C30" t="n">
+        <v>10</v>
+      </c>
+      <c r="D30" t="n">
+        <v>10</v>
+      </c>
+      <c r="E30" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>doc-5.2</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>8</v>
+      </c>
+      <c r="C31" t="n">
+        <v>8</v>
+      </c>
+      <c r="D31" t="n">
+        <v>8</v>
+      </c>
+      <c r="E31" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>doc-5.3</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>35</v>
+      </c>
+      <c r="C32" t="n">
+        <v>35</v>
+      </c>
+      <c r="D32" t="n">
+        <v>35</v>
+      </c>
+      <c r="E32" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>doc-5.4</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>16</v>
+      </c>
+      <c r="C33" t="n">
+        <v>16</v>
+      </c>
+      <c r="D33" t="n">
+        <v>16</v>
+      </c>
+      <c r="E33" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>doc-6.1</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>59</v>
+      </c>
+      <c r="C34" t="n">
+        <v>59</v>
+      </c>
+      <c r="D34" t="n">
+        <v>59</v>
+      </c>
+      <c r="E34" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>doc-6.2</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>4</v>
+      </c>
+      <c r="C35" t="n">
+        <v>4</v>
+      </c>
+      <c r="D35" t="n">
+        <v>4</v>
+      </c>
+      <c r="E35" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>doc-6.3</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>9</v>
+      </c>
+      <c r="C36" t="n">
+        <v>9</v>
+      </c>
+      <c r="D36" t="n">
+        <v>9</v>
+      </c>
+      <c r="E36" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>doc-7.1</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>8</v>
+      </c>
+      <c r="C37" t="n">
+        <v>8</v>
+      </c>
+      <c r="D37" t="n">
+        <v>8</v>
+      </c>
+      <c r="E37" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>doc-8.1</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>4</v>
+      </c>
+      <c r="C38" t="n">
+        <v>4</v>
+      </c>
+      <c r="D38" t="n">
+        <v>4</v>
+      </c>
+      <c r="E38" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>doc-8.2</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>9</v>
+      </c>
+      <c r="C39" t="n">
+        <v>9</v>
+      </c>
+      <c r="D39" t="n">
+        <v>9</v>
+      </c>
+      <c r="E39" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>doc-8.3</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>11</v>
+      </c>
+      <c r="C40" t="n">
+        <v>11</v>
+      </c>
+      <c r="D40" t="n">
+        <v>11</v>
+      </c>
+      <c r="E40" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>doc-9.1</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>20</v>
+      </c>
+      <c r="C41" t="n">
+        <v>20</v>
+      </c>
+      <c r="D41" t="n">
+        <v>20</v>
+      </c>
+      <c r="E41" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>doc-9.2</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>30</v>
+      </c>
+      <c r="C42" t="n">
+        <v>30</v>
+      </c>
+      <c r="D42" t="n">
+        <v>30</v>
+      </c>
+      <c r="E42" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>doc-9.3</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>8</v>
+      </c>
+      <c r="C43" t="n">
+        <v>8</v>
+      </c>
+      <c r="D43" t="n">
+        <v>8</v>
+      </c>
+      <c r="E43" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>doc-9.4</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>9</v>
+      </c>
+      <c r="C44" t="n">
+        <v>9</v>
+      </c>
+      <c r="D44" t="n">
+        <v>9</v>
+      </c>
+      <c r="E44" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>doc-9.5</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>23</v>
+      </c>
+      <c r="C45" t="n">
+        <v>23</v>
+      </c>
+      <c r="D45" t="n">
+        <v>23</v>
+      </c>
+      <c r="E45" t="n">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -787,16 +1670,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>22.09090909090909</v>
+        <v>22.5</v>
       </c>
       <c r="C3" t="n">
-        <v>22.09090909090909</v>
+        <v>22.5</v>
       </c>
       <c r="D3" t="n">
-        <v>22.09090909090909</v>
+        <v>22.5</v>
       </c>
       <c r="E3" t="n">
-        <v>22.09090909090909</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="4">
@@ -806,16 +1689,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>32.69721429128401</v>
+        <v>32.10194517036204</v>
       </c>
       <c r="C4" t="n">
-        <v>32.69721429128401</v>
+        <v>32.10194517036204</v>
       </c>
       <c r="D4" t="n">
-        <v>32.69721429128401</v>
+        <v>32.10194517036204</v>
       </c>
       <c r="E4" t="n">
-        <v>32.69721429128401</v>
+        <v>32.10194517036204</v>
       </c>
     </row>
     <row r="5">
@@ -882,16 +1765,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>20</v>
+        <v>20.75</v>
       </c>
       <c r="C8" t="n">
-        <v>20</v>
+        <v>20.75</v>
       </c>
       <c r="D8" t="n">
-        <v>20</v>
+        <v>20.75</v>
       </c>
       <c r="E8" t="n">
-        <v>20</v>
+        <v>20.75</v>
       </c>
     </row>
     <row r="9">
@@ -901,16 +1784,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C9" t="n">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="D9" t="n">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="E9" t="n">
-        <v>192</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
activity_relation_data_preparation: add non-related relations for the remaining activity pairs
</commit_message>
<xml_diff>
--- a/data/paper_stats/activity_relation/activity_relation_data_stats.xlsx
+++ b/data/paper_stats/activity_relation/activity_relation_data_stats.xlsx
@@ -9,8 +9,10 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Relation Type Count" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Comment Count" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Doc Count" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Doc Stats" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Doc Count Normal" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Doc Stats Normal" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Doc Count Non-related" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Doc Stats Non-related" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -449,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,12 +472,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>gateway_1</t>
+          <t>activity_1</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>gateway_2</t>
+          <t>activity_2</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -539,6 +541,25 @@
       </c>
       <c r="E4" t="n">
         <v>470</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>non_related</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2959</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2959</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2959</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2959</v>
       </c>
     </row>
   </sheetData>
@@ -552,7 +573,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -578,12 +599,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>gateway_1</t>
+          <t>activity_1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>gateway_2</t>
+          <t>activity_2</t>
         </is>
       </c>
     </row>
@@ -716,6 +737,23 @@
       </c>
       <c r="E8" t="n">
         <v>470</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>non_related</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>2959</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2959</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2959</v>
       </c>
     </row>
   </sheetData>
@@ -748,12 +786,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>gateway_1</t>
+          <t>activity_1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>gateway_2</t>
+          <t>activity_2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -1625,12 +1663,12 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>gateway_1</t>
+          <t>activity_1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>gateway_2</t>
+          <t>activity_2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -1794,6 +1832,1081 @@
       </c>
       <c r="E9" t="n">
         <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>doc_name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>activity_1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>activity_2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>relation_type</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>doc-1.1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>33</v>
+      </c>
+      <c r="C2" t="n">
+        <v>33</v>
+      </c>
+      <c r="D2" t="n">
+        <v>33</v>
+      </c>
+      <c r="E2" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>doc-1.2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>31</v>
+      </c>
+      <c r="C3" t="n">
+        <v>31</v>
+      </c>
+      <c r="D3" t="n">
+        <v>31</v>
+      </c>
+      <c r="E3" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>doc-1.3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>42</v>
+      </c>
+      <c r="C4" t="n">
+        <v>42</v>
+      </c>
+      <c r="D4" t="n">
+        <v>42</v>
+      </c>
+      <c r="E4" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>doc-1.4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>44</v>
+      </c>
+      <c r="C5" t="n">
+        <v>44</v>
+      </c>
+      <c r="D5" t="n">
+        <v>44</v>
+      </c>
+      <c r="E5" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.1</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.10</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>30</v>
+      </c>
+      <c r="C7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D7" t="n">
+        <v>30</v>
+      </c>
+      <c r="E7" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.11</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>18</v>
+      </c>
+      <c r="C8" t="n">
+        <v>18</v>
+      </c>
+      <c r="D8" t="n">
+        <v>18</v>
+      </c>
+      <c r="E8" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.12</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.13</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.14</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.2</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>72</v>
+      </c>
+      <c r="C12" t="n">
+        <v>72</v>
+      </c>
+      <c r="D12" t="n">
+        <v>72</v>
+      </c>
+      <c r="E12" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.3</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>36</v>
+      </c>
+      <c r="C13" t="n">
+        <v>36</v>
+      </c>
+      <c r="D13" t="n">
+        <v>36</v>
+      </c>
+      <c r="E13" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.4</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>35</v>
+      </c>
+      <c r="C14" t="n">
+        <v>35</v>
+      </c>
+      <c r="D14" t="n">
+        <v>35</v>
+      </c>
+      <c r="E14" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.5</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>6</v>
+      </c>
+      <c r="C15" t="n">
+        <v>6</v>
+      </c>
+      <c r="D15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E15" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.6</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" t="n">
+        <v>3</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.7</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>21</v>
+      </c>
+      <c r="C17" t="n">
+        <v>21</v>
+      </c>
+      <c r="D17" t="n">
+        <v>21</v>
+      </c>
+      <c r="E17" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.8</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>20</v>
+      </c>
+      <c r="C18" t="n">
+        <v>20</v>
+      </c>
+      <c r="D18" t="n">
+        <v>20</v>
+      </c>
+      <c r="E18" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>doc-10.9</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>16</v>
+      </c>
+      <c r="C19" t="n">
+        <v>16</v>
+      </c>
+      <c r="D19" t="n">
+        <v>16</v>
+      </c>
+      <c r="E19" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>doc-2.1</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>744</v>
+      </c>
+      <c r="C20" t="n">
+        <v>744</v>
+      </c>
+      <c r="D20" t="n">
+        <v>744</v>
+      </c>
+      <c r="E20" t="n">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>doc-2.2</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>302</v>
+      </c>
+      <c r="C21" t="n">
+        <v>302</v>
+      </c>
+      <c r="D21" t="n">
+        <v>302</v>
+      </c>
+      <c r="E21" t="n">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>doc-3.1</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>45</v>
+      </c>
+      <c r="C22" t="n">
+        <v>45</v>
+      </c>
+      <c r="D22" t="n">
+        <v>45</v>
+      </c>
+      <c r="E22" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>doc-3.2</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>5</v>
+      </c>
+      <c r="D23" t="n">
+        <v>5</v>
+      </c>
+      <c r="E23" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>doc-3.3</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>12</v>
+      </c>
+      <c r="C24" t="n">
+        <v>12</v>
+      </c>
+      <c r="D24" t="n">
+        <v>12</v>
+      </c>
+      <c r="E24" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>doc-3.5</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>102</v>
+      </c>
+      <c r="C25" t="n">
+        <v>102</v>
+      </c>
+      <c r="D25" t="n">
+        <v>102</v>
+      </c>
+      <c r="E25" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>doc-3.6</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>21</v>
+      </c>
+      <c r="C26" t="n">
+        <v>21</v>
+      </c>
+      <c r="D26" t="n">
+        <v>21</v>
+      </c>
+      <c r="E26" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>doc-3.7</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>10</v>
+      </c>
+      <c r="C27" t="n">
+        <v>10</v>
+      </c>
+      <c r="D27" t="n">
+        <v>10</v>
+      </c>
+      <c r="E27" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>doc-3.8</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>33</v>
+      </c>
+      <c r="C28" t="n">
+        <v>33</v>
+      </c>
+      <c r="D28" t="n">
+        <v>33</v>
+      </c>
+      <c r="E28" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>doc-4.1</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>558</v>
+      </c>
+      <c r="C29" t="n">
+        <v>558</v>
+      </c>
+      <c r="D29" t="n">
+        <v>558</v>
+      </c>
+      <c r="E29" t="n">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>doc-5.1</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>5</v>
+      </c>
+      <c r="C30" t="n">
+        <v>5</v>
+      </c>
+      <c r="D30" t="n">
+        <v>5</v>
+      </c>
+      <c r="E30" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>doc-5.2</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>13</v>
+      </c>
+      <c r="C31" t="n">
+        <v>13</v>
+      </c>
+      <c r="D31" t="n">
+        <v>13</v>
+      </c>
+      <c r="E31" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>doc-5.3</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>86</v>
+      </c>
+      <c r="C32" t="n">
+        <v>86</v>
+      </c>
+      <c r="D32" t="n">
+        <v>86</v>
+      </c>
+      <c r="E32" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>doc-5.4</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>30</v>
+      </c>
+      <c r="C33" t="n">
+        <v>30</v>
+      </c>
+      <c r="D33" t="n">
+        <v>30</v>
+      </c>
+      <c r="E33" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>doc-6.1</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>349</v>
+      </c>
+      <c r="C34" t="n">
+        <v>349</v>
+      </c>
+      <c r="D34" t="n">
+        <v>349</v>
+      </c>
+      <c r="E34" t="n">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>doc-6.2</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>6</v>
+      </c>
+      <c r="C35" t="n">
+        <v>6</v>
+      </c>
+      <c r="D35" t="n">
+        <v>6</v>
+      </c>
+      <c r="E35" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>doc-6.3</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>27</v>
+      </c>
+      <c r="C36" t="n">
+        <v>27</v>
+      </c>
+      <c r="D36" t="n">
+        <v>27</v>
+      </c>
+      <c r="E36" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>doc-7.1</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>13</v>
+      </c>
+      <c r="C37" t="n">
+        <v>13</v>
+      </c>
+      <c r="D37" t="n">
+        <v>13</v>
+      </c>
+      <c r="E37" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>doc-8.1</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>6</v>
+      </c>
+      <c r="C38" t="n">
+        <v>6</v>
+      </c>
+      <c r="D38" t="n">
+        <v>6</v>
+      </c>
+      <c r="E38" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>doc-8.2</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>27</v>
+      </c>
+      <c r="C39" t="n">
+        <v>27</v>
+      </c>
+      <c r="D39" t="n">
+        <v>27</v>
+      </c>
+      <c r="E39" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>doc-8.3</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>8</v>
+      </c>
+      <c r="C40" t="n">
+        <v>8</v>
+      </c>
+      <c r="D40" t="n">
+        <v>8</v>
+      </c>
+      <c r="E40" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>doc-9.1</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>25</v>
+      </c>
+      <c r="C41" t="n">
+        <v>25</v>
+      </c>
+      <c r="D41" t="n">
+        <v>25</v>
+      </c>
+      <c r="E41" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>doc-9.2</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>15</v>
+      </c>
+      <c r="C42" t="n">
+        <v>15</v>
+      </c>
+      <c r="D42" t="n">
+        <v>15</v>
+      </c>
+      <c r="E42" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>doc-9.3</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>28</v>
+      </c>
+      <c r="C43" t="n">
+        <v>28</v>
+      </c>
+      <c r="D43" t="n">
+        <v>28</v>
+      </c>
+      <c r="E43" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>doc-9.4</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>36</v>
+      </c>
+      <c r="C44" t="n">
+        <v>36</v>
+      </c>
+      <c r="D44" t="n">
+        <v>36</v>
+      </c>
+      <c r="E44" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>doc-9.5</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>28</v>
+      </c>
+      <c r="C45" t="n">
+        <v>28</v>
+      </c>
+      <c r="D45" t="n">
+        <v>28</v>
+      </c>
+      <c r="E45" t="n">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>activity_1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>activity_2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>relation_type</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>44</v>
+      </c>
+      <c r="C2" t="n">
+        <v>44</v>
+      </c>
+      <c r="D2" t="n">
+        <v>44</v>
+      </c>
+      <c r="E2" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>67.25</v>
+      </c>
+      <c r="C3" t="n">
+        <v>67.25</v>
+      </c>
+      <c r="D3" t="n">
+        <v>67.25</v>
+      </c>
+      <c r="E3" t="n">
+        <v>67.25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>std</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>146.5137702870312</v>
+      </c>
+      <c r="C4" t="n">
+        <v>146.5137702870312</v>
+      </c>
+      <c r="D4" t="n">
+        <v>146.5137702870312</v>
+      </c>
+      <c r="E4" t="n">
+        <v>146.5137702870312</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>25%</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>9.75</v>
+      </c>
+      <c r="C6" t="n">
+        <v>9.75</v>
+      </c>
+      <c r="D6" t="n">
+        <v>9.75</v>
+      </c>
+      <c r="E6" t="n">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>26</v>
+      </c>
+      <c r="C7" t="n">
+        <v>26</v>
+      </c>
+      <c r="D7" t="n">
+        <v>26</v>
+      </c>
+      <c r="E7" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>36</v>
+      </c>
+      <c r="C8" t="n">
+        <v>36</v>
+      </c>
+      <c r="D8" t="n">
+        <v>36</v>
+      </c>
+      <c r="E8" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>744</v>
+      </c>
+      <c r="C9" t="n">
+        <v>744</v>
+      </c>
+      <c r="D9" t="n">
+        <v>744</v>
+      </c>
+      <c r="E9" t="n">
+        <v>744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>